<commit_message>
New ontologies added (bill of material, currency, production, unit).
</commit_message>
<xml_diff>
--- a/ontology_tables/common_ontology.xlsx
+++ b/ontology_tables/common_ontology.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/q436477/Projekte/knowledge_agents/ontology/ontology_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0716853-CCA7-4046-8BE3-E7B8CAD187BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CBFB48-D412-9A4D-A959-7504AFC1D8C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="33840" windowHeight="21640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="322">
   <si>
     <t>type</t>
   </si>
@@ -103,12 +103,6 @@
     <t>automobile association</t>
   </si>
   <si>
-    <t>si base unit</t>
-  </si>
-  <si>
-    <t>si derived unit</t>
-  </si>
-  <si>
     <t>file format</t>
   </si>
   <si>
@@ -514,102 +508,6 @@
     <t>ISO name</t>
   </si>
   <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t>system of measurement</t>
-  </si>
-  <si>
-    <t>international system</t>
-  </si>
-  <si>
-    <t>second</t>
-  </si>
-  <si>
-    <t>metre</t>
-  </si>
-  <si>
-    <t>kilogram</t>
-  </si>
-  <si>
-    <t>ampere</t>
-  </si>
-  <si>
-    <t>kelvin</t>
-  </si>
-  <si>
-    <t>mole</t>
-  </si>
-  <si>
-    <t>candela</t>
-  </si>
-  <si>
-    <t>radian</t>
-  </si>
-  <si>
-    <t>steradian</t>
-  </si>
-  <si>
-    <t>hertz</t>
-  </si>
-  <si>
-    <t>newton</t>
-  </si>
-  <si>
-    <t>pascal</t>
-  </si>
-  <si>
-    <t>joule</t>
-  </si>
-  <si>
-    <t>watt</t>
-  </si>
-  <si>
-    <t>coulomb</t>
-  </si>
-  <si>
-    <t>volt</t>
-  </si>
-  <si>
-    <t>farad</t>
-  </si>
-  <si>
-    <t>ohm</t>
-  </si>
-  <si>
-    <t>siemens</t>
-  </si>
-  <si>
-    <t>weber</t>
-  </si>
-  <si>
-    <t>tesla</t>
-  </si>
-  <si>
-    <t>henry</t>
-  </si>
-  <si>
-    <t>degree Celsius</t>
-  </si>
-  <si>
-    <t>lumen</t>
-  </si>
-  <si>
-    <t>lux</t>
-  </si>
-  <si>
-    <t>becquerel</t>
-  </si>
-  <si>
-    <t>gray</t>
-  </si>
-  <si>
-    <t>sievert</t>
-  </si>
-  <si>
-    <t>katal</t>
-  </si>
-  <si>
     <t>skill</t>
   </si>
   <si>
@@ -790,9 +688,6 @@
     <t>Europäische Norm</t>
   </si>
   <si>
-    <t>Einheitensystem</t>
-  </si>
-  <si>
     <t>Vorschrift</t>
   </si>
   <si>
@@ -856,93 +751,6 @@
     <t>B2B</t>
   </si>
   <si>
-    <t>time, duration</t>
-  </si>
-  <si>
-    <t>length</t>
-  </si>
-  <si>
-    <t>mass</t>
-  </si>
-  <si>
-    <t>electric current</t>
-  </si>
-  <si>
-    <t>thermodynamic temperature</t>
-  </si>
-  <si>
-    <t>amount of substance</t>
-  </si>
-  <si>
-    <t>luminous intensity</t>
-  </si>
-  <si>
-    <t>plane angle</t>
-  </si>
-  <si>
-    <t>solid angle</t>
-  </si>
-  <si>
-    <t>frequency</t>
-  </si>
-  <si>
-    <t>force, weight</t>
-  </si>
-  <si>
-    <t>pressure, stress</t>
-  </si>
-  <si>
-    <t>energy, work, heat</t>
-  </si>
-  <si>
-    <t>power, radiant flux</t>
-  </si>
-  <si>
-    <t>electric charge</t>
-  </si>
-  <si>
-    <t>electrical potential difference (voltage), emf</t>
-  </si>
-  <si>
-    <t>capacitance</t>
-  </si>
-  <si>
-    <t>resistance, impedance, reactance</t>
-  </si>
-  <si>
-    <t>electrical conductance</t>
-  </si>
-  <si>
-    <t>magnetic flux</t>
-  </si>
-  <si>
-    <t>magnetic flux density</t>
-  </si>
-  <si>
-    <t>inductance</t>
-  </si>
-  <si>
-    <t>temperature relative to 273.15 K</t>
-  </si>
-  <si>
-    <t>luminous flux</t>
-  </si>
-  <si>
-    <t>illuminance</t>
-  </si>
-  <si>
-    <t>activity referred to a radionuclide (decays per unit time)</t>
-  </si>
-  <si>
-    <t>absorbed dose (of ionising radiation)</t>
-  </si>
-  <si>
-    <t>equivalent dose (of ionising radiation)</t>
-  </si>
-  <si>
-    <t>catalytic activity</t>
-  </si>
-  <si>
     <t>Asset Administration Shell (AAS), digital twin</t>
   </si>
   <si>
@@ -1000,96 +808,6 @@
     <t>International Organization for Standardization (ISO)</t>
   </si>
   <si>
-    <t>si system, international system of units</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>kg</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>mol</t>
-  </si>
-  <si>
-    <t>cd</t>
-  </si>
-  <si>
-    <t>rad</t>
-  </si>
-  <si>
-    <t>sr</t>
-  </si>
-  <si>
-    <t>Hz</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Pa</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>Ω</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>Wb</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>°C</t>
-  </si>
-  <si>
-    <t>lm</t>
-  </si>
-  <si>
-    <t>lx</t>
-  </si>
-  <si>
-    <t>Bq</t>
-  </si>
-  <si>
-    <t>Gy</t>
-  </si>
-  <si>
-    <t>Sv</t>
-  </si>
-  <si>
-    <t>kat</t>
-  </si>
-  <si>
     <t>Gesetz, Vorordnung</t>
   </si>
   <si>
@@ -1114,9 +832,6 @@
     <t>Allgemeiner Deutscher Automobilclub (ADAC)</t>
   </si>
   <si>
-    <t>SI System</t>
-  </si>
-  <si>
     <t>https://schema.org/price</t>
   </si>
   <si>
@@ -1247,42 +962,6 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/International_Organization_for_Standardization</t>
-  </si>
-  <si>
-    <t>https://schema.org/unitText, https://schema.org/unitCode</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/System_of_measurement</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/International_System_of_Units</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/International_System_of_Units#SI_base_units</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/International_System_of_Units#SI_derived_units</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Second</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Metre</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Kilogram</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Ampere</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Kelvin</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Mole_(unit)</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Candela</t>
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Regulation_(European_Union)</t>
@@ -1763,8 +1442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O313"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="E155" sqref="E155"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="E183" sqref="E183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1824,7 +1503,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -1832,7 +1511,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -1840,7 +1519,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -1848,7 +1527,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -1856,7 +1535,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -1869,7 +1548,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -1877,7 +1556,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>428</v>
+        <v>321</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -1885,13 +1564,13 @@
         <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -1899,13 +1578,13 @@
         <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -1917,13 +1596,13 @@
         <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -1931,13 +1610,13 @@
         <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -1945,13 +1624,13 @@
         <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
@@ -1959,13 +1638,13 @@
         <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>208</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
@@ -1973,16 +1652,16 @@
         <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>273</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
@@ -1990,13 +1669,13 @@
         <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
@@ -2004,16 +1683,16 @@
         <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>210</v>
+        <v>176</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>365</v>
+        <v>270</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
@@ -2021,28 +1700,28 @@
         <v>23</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>204</v>
+        <v>170</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>221</v>
+        <v>187</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>260</v>
+        <v>225</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>308</v>
+        <v>244</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>360</v>
+        <v>266</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>366</v>
+        <v>271</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
@@ -2050,22 +1729,22 @@
         <v>23</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>205</v>
+        <v>171</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>222</v>
+        <v>188</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>261</v>
+        <v>226</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>367</v>
+        <v>272</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
@@ -2073,10 +1752,10 @@
         <v>23</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
@@ -2084,10 +1763,10 @@
         <v>23</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
@@ -2095,16 +1774,16 @@
         <v>23</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>223</v>
+        <v>189</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>368</v>
+        <v>273</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
@@ -2112,13 +1791,13 @@
         <v>23</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>224</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
@@ -2126,13 +1805,13 @@
         <v>23</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
@@ -2140,16 +1819,16 @@
         <v>23</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>226</v>
+        <v>192</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>369</v>
+        <v>274</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
@@ -2157,13 +1836,13 @@
         <v>24</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
@@ -2171,16 +1850,16 @@
         <v>23</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>227</v>
+        <v>193</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>370</v>
+        <v>275</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
@@ -2188,22 +1867,22 @@
         <v>23</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>228</v>
+        <v>194</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>309</v>
+        <v>245</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>361</v>
+        <v>267</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>371</v>
+        <v>276</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
@@ -2211,25 +1890,25 @@
         <v>23</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>229</v>
+        <v>195</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>262</v>
+        <v>227</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>274</v>
+        <v>239</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>310</v>
+        <v>246</v>
       </c>
       <c r="M48" s="3" t="s">
-        <v>372</v>
+        <v>277</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
@@ -2237,22 +1916,22 @@
         <v>24</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>212</v>
+        <v>178</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>263</v>
+        <v>228</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>311</v>
+        <v>247</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
@@ -2260,19 +1939,19 @@
         <v>24</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>213</v>
+        <v>179</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>264</v>
+        <v>229</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
@@ -2280,13 +1959,13 @@
         <v>25</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
@@ -2294,13 +1973,13 @@
         <v>25</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
@@ -2308,13 +1987,13 @@
         <v>23</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>265</v>
+        <v>230</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
@@ -2322,16 +2001,16 @@
         <v>25</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>266</v>
+        <v>231</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
@@ -2339,13 +2018,13 @@
         <v>25</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
@@ -2353,16 +2032,16 @@
         <v>23</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>230</v>
+        <v>196</v>
       </c>
       <c r="M58" s="3" t="s">
-        <v>373</v>
+        <v>278</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
@@ -2370,13 +2049,13 @@
         <v>25</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
@@ -2384,13 +2063,13 @@
         <v>24</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
@@ -2398,16 +2077,16 @@
         <v>23</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>231</v>
+        <v>197</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>374</v>
+        <v>279</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
@@ -2415,13 +2094,13 @@
         <v>25</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
@@ -2429,13 +2108,13 @@
         <v>25</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
@@ -2443,13 +2122,13 @@
         <v>24</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
@@ -2457,13 +2136,13 @@
         <v>24</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
@@ -2471,13 +2150,13 @@
         <v>23</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>232</v>
+        <v>198</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
@@ -2485,13 +2164,13 @@
         <v>25</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
@@ -2499,13 +2178,13 @@
         <v>25</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
@@ -2513,19 +2192,19 @@
         <v>23</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>233</v>
+        <v>199</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>312</v>
+        <v>248</v>
       </c>
       <c r="L73" s="1" t="s">
-        <v>362</v>
+        <v>268</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
@@ -2533,13 +2212,13 @@
         <v>25</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D74" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="E74" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
@@ -2547,13 +2226,13 @@
         <v>24</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
@@ -2561,16 +2240,16 @@
         <v>23</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>234</v>
+        <v>200</v>
       </c>
       <c r="M77" s="3" t="s">
-        <v>375</v>
+        <v>280</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
@@ -2578,13 +2257,13 @@
         <v>23</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>235</v>
+        <v>201</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.2">
@@ -2592,19 +2271,19 @@
         <v>23</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>236</v>
+        <v>202</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>313</v>
+        <v>249</v>
       </c>
       <c r="M80" s="3" t="s">
-        <v>376</v>
+        <v>281</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.2">
@@ -2612,13 +2291,13 @@
         <v>25</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.2">
@@ -2626,13 +2305,13 @@
         <v>25</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.2">
@@ -2640,13 +2319,13 @@
         <v>24</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.2">
@@ -2654,13 +2333,13 @@
         <v>24</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.2">
@@ -2668,13 +2347,13 @@
         <v>23</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.2">
@@ -2682,19 +2361,19 @@
         <v>23</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>238</v>
+        <v>204</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>314</v>
+        <v>250</v>
       </c>
       <c r="M89" s="3" t="s">
-        <v>377</v>
+        <v>282</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.2">
@@ -2702,13 +2381,13 @@
         <v>25</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.2">
@@ -2716,22 +2395,22 @@
         <v>23</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>239</v>
+        <v>205</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>276</v>
+        <v>241</v>
       </c>
       <c r="M92" s="3" t="s">
-        <v>378</v>
+        <v>283</v>
       </c>
       <c r="O92" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.2">
@@ -2739,13 +2418,13 @@
         <v>25</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.2">
@@ -2753,22 +2432,22 @@
         <v>23</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>240</v>
+        <v>206</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>277</v>
+        <v>242</v>
       </c>
       <c r="M95" s="3" t="s">
-        <v>379</v>
+        <v>284</v>
       </c>
       <c r="O95" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.2">
@@ -2776,13 +2455,13 @@
         <v>25</v>
       </c>
       <c r="B96" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D96" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="E96" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">
@@ -2790,16 +2469,16 @@
         <v>23</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>241</v>
+        <v>207</v>
       </c>
       <c r="M98" s="3" t="s">
-        <v>380</v>
+        <v>285</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.2">
@@ -2807,13 +2486,13 @@
         <v>25</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.2">
@@ -2821,16 +2500,16 @@
         <v>23</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>242</v>
+        <v>208</v>
       </c>
       <c r="M101" s="3" t="s">
-        <v>381</v>
+        <v>286</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
@@ -2838,13 +2517,13 @@
         <v>25</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
@@ -2852,13 +2531,13 @@
         <v>23</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>243</v>
+        <v>209</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.2">
@@ -2866,13 +2545,13 @@
         <v>25</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.2">
@@ -2880,16 +2559,16 @@
         <v>23</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K107" s="1" t="s">
-        <v>315</v>
+        <v>251</v>
       </c>
       <c r="M107" s="3" t="s">
-        <v>382</v>
+        <v>287</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
@@ -2897,16 +2576,16 @@
         <v>25</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M108" s="3" t="s">
-        <v>383</v>
+        <v>288</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
@@ -2914,16 +2593,16 @@
         <v>25</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
       <c r="M109" s="3" t="s">
-        <v>384</v>
+        <v>289</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
@@ -2931,13 +2610,13 @@
         <v>23</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M111" s="3" t="s">
-        <v>385</v>
+        <v>290</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.2">
@@ -2945,10 +2624,10 @@
         <v>23</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.2">
@@ -2956,10 +2635,10 @@
         <v>23</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.2">
@@ -2967,16 +2646,16 @@
         <v>23</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>244</v>
+        <v>210</v>
       </c>
       <c r="M117" s="3" t="s">
-        <v>386</v>
+        <v>291</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.2">
@@ -2984,16 +2663,16 @@
         <v>23</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>245</v>
+        <v>211</v>
       </c>
       <c r="M119" s="3" t="s">
-        <v>387</v>
+        <v>292</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.2">
@@ -3001,13 +2680,13 @@
         <v>23</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M123" s="3" t="s">
-        <v>388</v>
+        <v>293</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.2">
@@ -3015,13 +2694,13 @@
         <v>23</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M124" s="3" t="s">
-        <v>389</v>
+        <v>294</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.2">
@@ -3029,22 +2708,22 @@
         <v>23</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>246</v>
+        <v>212</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="K125" s="1" t="s">
-        <v>316</v>
+        <v>252</v>
       </c>
       <c r="M125" s="3" t="s">
-        <v>390</v>
+        <v>295</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.2">
@@ -3052,22 +2731,22 @@
         <v>23</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>247</v>
+        <v>213</v>
       </c>
       <c r="H126" s="1" t="s">
-        <v>268</v>
+        <v>233</v>
       </c>
       <c r="K126" s="1" t="s">
-        <v>317</v>
+        <v>253</v>
       </c>
       <c r="M126" s="3" t="s">
-        <v>391</v>
+        <v>296</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.2">
@@ -3075,16 +2754,16 @@
         <v>23</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K127" s="1" t="s">
-        <v>318</v>
+        <v>254</v>
       </c>
       <c r="M127" s="3" t="s">
-        <v>392</v>
+        <v>297</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.2">
@@ -3092,16 +2771,16 @@
         <v>23</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>269</v>
+        <v>234</v>
       </c>
       <c r="M128" s="3" t="s">
-        <v>393</v>
+        <v>298</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.2">
@@ -3109,13 +2788,13 @@
         <v>23</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>248</v>
+        <v>214</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.2">
@@ -3123,13 +2802,13 @@
         <v>23</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M132" s="3" t="s">
-        <v>394</v>
+        <v>299</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.2">
@@ -3137,13 +2816,13 @@
         <v>25</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.2">
@@ -3151,13 +2830,13 @@
         <v>23</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M134" s="3" t="s">
-        <v>395</v>
+        <v>300</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.2">
@@ -3165,13 +2844,13 @@
         <v>25</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.2">
@@ -3179,16 +2858,16 @@
         <v>23</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>249</v>
+        <v>215</v>
       </c>
       <c r="M136" s="3" t="s">
-        <v>396</v>
+        <v>301</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.2">
@@ -3196,13 +2875,13 @@
         <v>25</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.2">
@@ -3213,13 +2892,13 @@
         <v>26</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>250</v>
+        <v>216</v>
       </c>
       <c r="M138" s="3" t="s">
-        <v>397</v>
+        <v>302</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.2">
@@ -3227,19 +2906,19 @@
         <v>26</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>214</v>
+        <v>180</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>214</v>
+        <v>180</v>
       </c>
       <c r="L139" s="1" t="s">
-        <v>363</v>
+        <v>269</v>
       </c>
       <c r="M139" s="3" t="s">
-        <v>398</v>
+        <v>303</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.2">
@@ -3247,13 +2926,13 @@
         <v>26</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K140" s="1" t="s">
-        <v>319</v>
+        <v>255</v>
       </c>
       <c r="M140" s="3" t="s">
-        <v>399</v>
+        <v>304</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.2">
@@ -3261,13 +2940,13 @@
         <v>23</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M142" s="3" t="s">
-        <v>400</v>
+        <v>305</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.2">
@@ -3275,13 +2954,13 @@
         <v>25</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.2">
@@ -3289,10 +2968,10 @@
         <v>23</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.2">
@@ -3300,13 +2979,13 @@
         <v>25</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.2">
@@ -3314,13 +2993,13 @@
         <v>23</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>251</v>
+        <v>217</v>
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.2">
@@ -3328,13 +3007,13 @@
         <v>25</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.2">
@@ -3342,13 +3021,13 @@
         <v>23</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>252</v>
+        <v>218</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.2">
@@ -3356,13 +3035,13 @@
         <v>25</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.2">
@@ -3370,13 +3049,13 @@
         <v>23</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>253</v>
+        <v>219</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.2">
@@ -3384,13 +3063,13 @@
         <v>25</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.2">
@@ -3398,13 +3077,13 @@
         <v>23</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>254</v>
+        <v>220</v>
       </c>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.2">
@@ -3412,13 +3091,13 @@
         <v>25</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>211</v>
+        <v>177</v>
       </c>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.2">
@@ -3426,10 +3105,10 @@
         <v>23</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.2">
@@ -3437,19 +3116,19 @@
         <v>23</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>215</v>
+        <v>181</v>
       </c>
       <c r="K159" s="1" t="s">
-        <v>320</v>
+        <v>256</v>
       </c>
       <c r="M159" s="3" t="s">
-        <v>401</v>
+        <v>306</v>
       </c>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.2">
@@ -3457,16 +3136,16 @@
         <v>24</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>216</v>
+        <v>182</v>
       </c>
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.2">
@@ -3474,16 +3153,16 @@
         <v>24</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>217</v>
+        <v>183</v>
       </c>
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.2">
@@ -3491,13 +3170,13 @@
         <v>23</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M163" s="3" t="s">
-        <v>402</v>
+        <v>307</v>
       </c>
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.2">
@@ -3505,16 +3184,16 @@
         <v>23</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K164" s="1" t="s">
-        <v>321</v>
+        <v>257</v>
       </c>
       <c r="M164" s="3" t="s">
-        <v>403</v>
+        <v>308</v>
       </c>
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.2">
@@ -3522,13 +3201,13 @@
         <v>23</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K166" s="1" t="s">
-        <v>322</v>
+        <v>258</v>
       </c>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.2">
@@ -3536,10 +3215,10 @@
         <v>23</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.2">
@@ -3547,10 +3226,10 @@
         <v>23</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.2">
@@ -3558,10 +3237,10 @@
         <v>23</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.2">
@@ -3569,13 +3248,13 @@
         <v>23</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I172" s="1" t="s">
-        <v>214</v>
+        <v>180</v>
       </c>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.2">
@@ -3583,13 +3262,13 @@
         <v>23</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I173" s="1" t="s">
-        <v>275</v>
+        <v>240</v>
       </c>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.2">
@@ -3597,10 +3276,10 @@
         <v>23</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
@@ -3608,10 +3287,10 @@
         <v>23</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
@@ -3619,10 +3298,10 @@
         <v>23</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
@@ -3630,10 +3309,10 @@
         <v>23</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
@@ -3641,10 +3320,10 @@
         <v>23</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
@@ -3652,10 +3331,10 @@
         <v>23</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="196" spans="1:13" x14ac:dyDescent="0.2">
@@ -3663,13 +3342,13 @@
         <v>23</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H196" s="1" t="s">
-        <v>270</v>
+        <v>235</v>
       </c>
     </row>
     <row r="198" spans="1:13" x14ac:dyDescent="0.2">
@@ -3677,13 +3356,13 @@
         <v>23</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M198" s="3" t="s">
-        <v>404</v>
+        <v>309</v>
       </c>
     </row>
     <row r="199" spans="1:13" x14ac:dyDescent="0.2">
@@ -3691,13 +3370,13 @@
         <v>24</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.2">
@@ -3705,13 +3384,13 @@
         <v>24</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="202" spans="1:13" x14ac:dyDescent="0.2">
@@ -3719,13 +3398,13 @@
         <v>23</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M202" s="3" t="s">
-        <v>405</v>
+        <v>310</v>
       </c>
     </row>
     <row r="204" spans="1:13" x14ac:dyDescent="0.2">
@@ -3733,16 +3412,16 @@
         <v>23</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K204" s="1" t="s">
-        <v>323</v>
+        <v>259</v>
       </c>
       <c r="M204" s="3" t="s">
-        <v>406</v>
+        <v>311</v>
       </c>
     </row>
     <row r="205" spans="1:13" x14ac:dyDescent="0.2">
@@ -3750,13 +3429,13 @@
         <v>24</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="206" spans="1:13" x14ac:dyDescent="0.2">
@@ -3764,13 +3443,13 @@
         <v>24</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="208" spans="1:13" x14ac:dyDescent="0.2">
@@ -3778,19 +3457,19 @@
         <v>23</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G208" s="1" t="s">
-        <v>255</v>
+        <v>221</v>
       </c>
       <c r="K208" s="1" t="s">
-        <v>324</v>
+        <v>260</v>
       </c>
       <c r="M208" s="3" t="s">
-        <v>407</v>
+        <v>312</v>
       </c>
     </row>
     <row r="209" spans="1:13" x14ac:dyDescent="0.2">
@@ -3798,13 +3477,13 @@
         <v>24</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="210" spans="1:13" x14ac:dyDescent="0.2">
@@ -3812,13 +3491,13 @@
         <v>24</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="212" spans="1:13" x14ac:dyDescent="0.2">
@@ -3826,16 +3505,16 @@
         <v>23</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K212" s="1" t="s">
-        <v>325</v>
+        <v>261</v>
       </c>
       <c r="M212" s="3" t="s">
-        <v>408</v>
+        <v>313</v>
       </c>
     </row>
     <row r="213" spans="1:13" x14ac:dyDescent="0.2">
@@ -3843,13 +3522,13 @@
         <v>24</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="214" spans="1:13" x14ac:dyDescent="0.2">
@@ -3857,530 +3536,60 @@
         <v>24</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="251" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A251" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B251" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C251" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M251" s="3" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A252" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B252" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C252" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G252" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="M252" s="3" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A253" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B253" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C253" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="K253" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="L253" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="M253" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A254" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B254" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C254" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="M254" s="3" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A255" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B255" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C255" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="M255" s="3" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A257" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B257" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="J257" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="K257" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="M257" s="3" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A258" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B258" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="J258" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K258" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="M258" s="3" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A259" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B259" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J259" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="K259" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="M259" s="3" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="260" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A260" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B260" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="J260" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="K260" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="M260" s="3" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="261" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A261" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B261" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="J261" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="K261" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="M261" s="3" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="262" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A262" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B262" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J262" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="K262" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="M262" s="3" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="263" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A263" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B263" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="J263" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="K263" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="M263" s="3" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A265" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B265" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="J265" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="K265" s="1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="266" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A266" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B266" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="J266" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="K266" s="1" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="267" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A267" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B267" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="J267" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="K267" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="268" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A268" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B268" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="J268" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="K268" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="269" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A269" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B269" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="J269" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="K269" s="1" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A270" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B270" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="J270" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="K270" s="1" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="271" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A271" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B271" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="J271" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="K271" s="1" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="272" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A272" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B272" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="J272" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="K272" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A273" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B273" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="J273" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="K273" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A274" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B274" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="J274" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="K274" s="1" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A275" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B275" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="J275" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="K275" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A276" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B276" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="J276" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="K276" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A277" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B277" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="J277" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="K277" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A278" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B278" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="J278" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="K278" s="1" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A279" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B279" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="J279" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="K279" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A280" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B280" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="J280" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="K280" s="1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A281" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B281" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="J281" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="K281" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A282" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B282" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="J282" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="K282" s="1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A283" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B283" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="J283" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="K283" s="1" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A284" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B284" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="J284" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="K284" s="1" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A285" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B285" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="J285" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="K285" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A286" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B286" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="J286" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="K286" s="1" t="s">
-        <v>355</v>
-      </c>
+    </row>
+    <row r="251" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M251" s="3"/>
+    </row>
+    <row r="252" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M252" s="3"/>
+    </row>
+    <row r="253" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M253" s="3"/>
+    </row>
+    <row r="254" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M254" s="3"/>
+    </row>
+    <row r="255" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M255" s="3"/>
+    </row>
+    <row r="257" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M257" s="3"/>
+    </row>
+    <row r="258" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M258" s="3"/>
+    </row>
+    <row r="259" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M259" s="3"/>
+    </row>
+    <row r="260" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M260" s="3"/>
+    </row>
+    <row r="261" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M261" s="3"/>
+    </row>
+    <row r="262" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M262" s="3"/>
+    </row>
+    <row r="263" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M263" s="3"/>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A302" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>196</v>
+        <v>162</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.2">
@@ -4388,10 +3597,10 @@
         <v>23</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="C303" s="1" t="s">
-        <v>196</v>
+        <v>162</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.2">
@@ -4399,10 +3608,10 @@
         <v>23</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="306" spans="1:13" x14ac:dyDescent="0.2">
@@ -4410,133 +3619,133 @@
         <v>23</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C306" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G306" s="1" t="s">
-        <v>257</v>
+        <v>222</v>
       </c>
       <c r="K306" s="1" t="s">
-        <v>356</v>
+        <v>262</v>
       </c>
       <c r="M306" s="3" t="s">
-        <v>421</v>
+        <v>314</v>
       </c>
     </row>
     <row r="308" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A308" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>198</v>
+        <v>164</v>
       </c>
       <c r="F308" s="1" t="s">
-        <v>218</v>
+        <v>184</v>
       </c>
       <c r="G308" s="1" t="s">
-        <v>218</v>
+        <v>184</v>
       </c>
       <c r="M308" s="3" t="s">
-        <v>422</v>
+        <v>315</v>
       </c>
     </row>
     <row r="309" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A309" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>199</v>
+        <v>165</v>
       </c>
       <c r="F309" s="1" t="s">
-        <v>199</v>
+        <v>165</v>
       </c>
       <c r="G309" s="1" t="s">
-        <v>199</v>
+        <v>165</v>
       </c>
       <c r="M309" s="3" t="s">
-        <v>423</v>
+        <v>316</v>
       </c>
     </row>
     <row r="310" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A310" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>200</v>
+        <v>166</v>
       </c>
       <c r="F310" s="1" t="s">
-        <v>219</v>
+        <v>185</v>
       </c>
       <c r="G310" s="1" t="s">
-        <v>219</v>
+        <v>185</v>
       </c>
       <c r="K310" s="1" t="s">
-        <v>357</v>
+        <v>263</v>
       </c>
       <c r="M310" s="3" t="s">
-        <v>424</v>
+        <v>317</v>
       </c>
     </row>
     <row r="311" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A311" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>201</v>
+        <v>167</v>
       </c>
       <c r="F311" s="1" t="s">
-        <v>220</v>
+        <v>186</v>
       </c>
       <c r="G311" s="1" t="s">
-        <v>220</v>
+        <v>186</v>
       </c>
       <c r="K311" s="1" t="s">
-        <v>358</v>
+        <v>264</v>
       </c>
       <c r="M311" s="3" t="s">
-        <v>425</v>
+        <v>318</v>
       </c>
     </row>
     <row r="312" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A312" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>202</v>
+        <v>168</v>
       </c>
       <c r="G312" s="1" t="s">
-        <v>258</v>
+        <v>223</v>
       </c>
       <c r="H312" s="1" t="s">
-        <v>271</v>
+        <v>236</v>
       </c>
       <c r="J312" s="1" t="s">
-        <v>307</v>
+        <v>243</v>
       </c>
       <c r="K312" s="1" t="s">
-        <v>359</v>
+        <v>265</v>
       </c>
       <c r="M312" s="3" t="s">
-        <v>426</v>
+        <v>319</v>
       </c>
     </row>
     <row r="313" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A313" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>203</v>
+        <v>169</v>
       </c>
       <c r="G313" s="1" t="s">
-        <v>259</v>
+        <v>224</v>
       </c>
       <c r="H313" s="1" t="s">
-        <v>272</v>
+        <v>237</v>
       </c>
       <c r="M313" s="3" t="s">
-        <v>427</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -4605,25 +3814,13 @@
     <hyperlink ref="M204" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
     <hyperlink ref="M208" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
     <hyperlink ref="M212" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="M251" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="M252" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="M253" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="M254" r:id="rId46" location="SI_base_units" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="M255" r:id="rId47" location="SI_derived_units" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="M257" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="M258" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="M259" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="M260" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="M261" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="M262" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="M263" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="M306" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="M308" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="M309" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="M310" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="M311" r:id="rId59" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="M312" r:id="rId60" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="M313" r:id="rId61" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="M306" r:id="rId43" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="M308" r:id="rId44" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="M309" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="M310" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="M311" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="M312" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="M313" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>